<commit_message>
Fix arrondie <etat virement>
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_7_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_7_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +423,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>147/123456</v>
+        <v>910/TANGER /AV1</v>
       </c>
       <c r="B2" t="str">
-        <v>Siège</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>DE56468</v>
+        <v>D235689</v>
       </c>
       <c r="D2" t="str">
-        <v>MOHAMED ALMAKTOM</v>
+        <v>KAMILIA LALA</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -444,77 +444,77 @@
         <v>15</v>
       </c>
       <c r="H2">
-        <v>10000</v>
+        <v>24000</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>24000</v>
       </c>
       <c r="J2">
-        <v>1500</v>
+        <v>3600</v>
       </c>
       <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
+        <v>3600</v>
+      </c>
+      <c r="L2" t="str">
+        <v>--</v>
       </c>
       <c r="M2">
-        <v>8500</v>
+        <v>20400</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>966/PV TEST</v>
+        <v>910/TANGER /AV1</v>
       </c>
       <c r="B3" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C3" t="str">
-        <v>545444</v>
+        <v>K3544354</v>
       </c>
       <c r="D3" t="str">
-        <v>Ali expresse</v>
+        <v>ABDOU FAFA</v>
       </c>
       <c r="E3" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F3" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
+        <v>15</v>
+      </c>
+      <c r="H3">
+        <v>13354.4</v>
+      </c>
+      <c r="I3">
+        <v>13354.4</v>
+      </c>
+      <c r="J3">
+        <v>2003.16</v>
+      </c>
+      <c r="K3">
+        <v>2003.16</v>
+      </c>
+      <c r="L3" t="str">
         <v>--</v>
       </c>
-      <c r="I3">
-        <v>91989.19</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>91989.19</v>
-      </c>
       <c r="M3">
-        <v>183978.39</v>
+        <v>11351.24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>966/PV TEST</v>
+        <v>910/TANGER /AV1</v>
       </c>
       <c r="B4" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>aq5146</v>
+        <v>L254654</v>
       </c>
       <c r="D4" t="str">
-        <v>Mohamed Amine</v>
+        <v>SAMIR DADA</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -523,39 +523,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>15</v>
-      </c>
-      <c r="H4" t="str">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>2645.6</v>
+      </c>
+      <c r="I4">
+        <v>2645.6</v>
+      </c>
+      <c r="J4">
+        <v>264.56</v>
+      </c>
+      <c r="K4">
+        <v>264.56</v>
+      </c>
+      <c r="L4" t="str">
         <v>--</v>
       </c>
-      <c r="I4">
-        <v>68010.93</v>
-      </c>
-      <c r="J4" t="str">
-        <v>--</v>
-      </c>
-      <c r="K4">
-        <v>10201.64</v>
-      </c>
-      <c r="L4">
-        <v>68010.93</v>
-      </c>
       <c r="M4">
-        <v>125820.22</v>
+        <v>2381.04</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>096/TEST</v>
+        <v>115/TANGER MED/AV1</v>
       </c>
       <c r="B5" t="str">
-        <v>Siège</v>
+        <v>Point de vente</v>
       </c>
       <c r="C5" t="str">
-        <v>q666465</v>
+        <v>L5245475</v>
       </c>
       <c r="D5" t="str">
-        <v>Ali Benani</v>
+        <v>MORAD JOJO</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -564,39 +564,39 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H5">
-        <v>45376.46</v>
+        <v>9000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>6806.47</v>
+        <v>900</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>0</v>
+      <c r="L5" t="str">
+        <v>--</v>
       </c>
       <c r="M5">
-        <v>38569.99</v>
+        <v>8100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>096/TEST</v>
+        <v>115/TANGER MED/AV1</v>
       </c>
       <c r="B6" t="str">
-        <v>Siège</v>
+        <v>Point de vente</v>
       </c>
       <c r="C6" t="str">
-        <v>aq46545</v>
+        <v>Z213568</v>
       </c>
       <c r="D6" t="str">
-        <v>Amine Mokhtar</v>
+        <v>NABIL MOMO</v>
       </c>
       <c r="E6" t="str">
         <v>non</v>
@@ -605,71 +605,194 @@
         <v>mensuelle</v>
       </c>
       <c r="G6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>14623.54</v>
+        <v>6000</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>2193.53</v>
+        <v>600</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
-      <c r="L6">
-        <v>0</v>
+      <c r="L6" t="str">
+        <v>--</v>
       </c>
       <c r="M6">
-        <v>12430.01</v>
+        <v>5400</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
+        <v>115/TANGER MED/AV1</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C7" t="str">
+        <v>L525655</v>
+      </c>
+      <c r="D7" t="str">
+        <v>KHALID RARA</v>
+      </c>
+      <c r="E7" t="str">
+        <v>non</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>6000</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>600</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7" t="str">
+        <v>--</v>
+      </c>
+      <c r="M7">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>844/T-SUD</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C8" t="str">
+        <v>K324554</v>
+      </c>
+      <c r="D8" t="str">
+        <v>KARIMA SASA</v>
+      </c>
+      <c r="E8" t="str">
+        <v>non</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8">
+        <v>24000</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>3600</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8" t="str">
+        <v>--</v>
+      </c>
+      <c r="M8">
+        <v>20400</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>844/T-SUD</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C9" t="str">
+        <v>IL12254</v>
+      </c>
+      <c r="D9" t="str">
+        <v>FARIDA VAVA</v>
+      </c>
+      <c r="E9" t="str">
+        <v>non</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>6000</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>600</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" t="str">
+        <v>--</v>
+      </c>
+      <c r="M9">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B7" t="str">
+      <c r="B10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C7" t="str">
+      <c r="C10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D7" t="str">
+      <c r="D10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E7" t="str">
+      <c r="E10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F7" t="str">
+      <c r="F10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G7" t="str">
+      <c r="G10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H7">
-        <v>70000</v>
-      </c>
-      <c r="I7">
-        <v>160000.12</v>
-      </c>
-      <c r="J7">
-        <v>10500</v>
-      </c>
-      <c r="K7">
-        <v>10201.64</v>
-      </c>
-      <c r="L7">
-        <v>160000.12</v>
-      </c>
-      <c r="M7">
-        <v>369298.61</v>
+      <c r="H10">
+        <v>91000</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>12167.72</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>78832.28</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:M7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:M10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix rappel (avance > duree rappel) issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_7_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_7_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,13 +415,13 @@
         <v>Taxe/avance</v>
       </c>
       <c r="L1" t="str">
+        <v>MT brut (Rappel)</v>
+      </c>
+      <c r="M1" t="str">
+        <v>Taxe (Rappel)</v>
+      </c>
+      <c r="N1" t="str">
         <v>Caution</v>
-      </c>
-      <c r="M1" t="str">
-        <v>MT brut (Rappel)</v>
-      </c>
-      <c r="N1" t="str">
-        <v>Taxe (Rappel)</v>
       </c>
       <c r="O1" t="str">
         <v>MT net</v>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>332/AG FES1</v>
+        <v>554/SUP FES 1</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Supervision</v>
       </c>
       <c r="C2" t="str">
-        <v>LK354534</v>
+        <v>D524564</v>
       </c>
       <c r="D2" t="str">
-        <v>MOURAD VAVA</v>
+        <v>SAMIRA TATA</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -453,39 +453,39 @@
         <v>--</v>
       </c>
       <c r="I2">
-        <v>48000</v>
+        <v>40000</v>
       </c>
       <c r="J2" t="str">
         <v>--</v>
       </c>
       <c r="K2">
-        <v>7200</v>
+        <v>6000</v>
       </c>
       <c r="L2">
-        <v>48000</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>7200</v>
-      </c>
-      <c r="N2" t="str">
-        <v>--</v>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>10000</v>
       </c>
       <c r="O2">
-        <v>40800</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>332/AG FES1</v>
+        <v xml:space="preserve">044/LF/FES VILLE </v>
       </c>
       <c r="B3" t="str">
-        <v>Point de vente</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C3" t="str">
-        <v>LK354534</v>
+        <v>L3578354</v>
       </c>
       <c r="D3" t="str">
-        <v>MOURAD VAVA</v>
+        <v>NABIL KAMAL</v>
       </c>
       <c r="E3" t="str">
         <v>non</v>
@@ -496,17 +496,17 @@
       <c r="G3">
         <v>15</v>
       </c>
-      <c r="H3">
-        <v>16000</v>
+      <c r="H3" t="str">
+        <v>--</v>
       </c>
       <c r="I3">
-        <v>48000</v>
-      </c>
-      <c r="J3">
-        <v>2400</v>
+        <v>40000</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
       </c>
       <c r="K3">
-        <v>7200</v>
+        <v>6000</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -515,24 +515,24 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>16000</v>
+        <v>10000</v>
       </c>
       <c r="O3">
-        <v>29600</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>966/RABAT SUP1</v>
+        <v xml:space="preserve">044/FES VILLE </v>
       </c>
       <c r="B4" t="str">
-        <v>Supervision</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C4" t="str">
-        <v>L5453746</v>
+        <v>K5443645</v>
       </c>
       <c r="D4" t="str">
-        <v>MERYEM RARA</v>
+        <v>KHADIJA LALA</v>
       </c>
       <c r="E4" t="str">
         <v>non</v>
@@ -541,45 +541,45 @@
         <v>mensuelle</v>
       </c>
       <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>2400</v>
+        <v>15</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4">
-        <v>0</v>
+      <c r="J4" t="str">
+        <v>--</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>9000</v>
       </c>
       <c r="N4" t="str">
         <v>--</v>
       </c>
       <c r="O4">
-        <v>2400</v>
+        <v>51000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>966/RABAT SUP1</v>
+        <v xml:space="preserve">044/FES VILLE </v>
       </c>
       <c r="B5" t="str">
-        <v>Supervision</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C5" t="str">
-        <v>KL254545</v>
+        <v>K5443645</v>
       </c>
       <c r="D5" t="str">
-        <v>LAILA JJJJ</v>
+        <v>KHADIJA LALA</v>
       </c>
       <c r="E5" t="str">
         <v>non</v>
@@ -588,16 +588,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H5">
-        <v>3600</v>
+        <v>10000</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
       <c r="J5">
-        <v>360</v>
+        <v>1500</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -608,251 +608,63 @@
       <c r="M5">
         <v>0</v>
       </c>
-      <c r="N5" t="str">
-        <v>--</v>
+      <c r="N5">
+        <v>10000</v>
       </c>
       <c r="O5">
-        <v>3240</v>
+        <v>18500</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>966/RABAT SUP1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B6" t="str">
-        <v>Supervision</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C6" t="str">
-        <v>M6346854</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D6" t="str">
-        <v xml:space="preserve">SAMIA NARA </v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E6" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G6" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H6">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="J6">
-        <v>600</v>
+        <v>1500</v>
       </c>
       <c r="K6">
-        <v>0</v>
+        <v>12000</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>60000</v>
       </c>
       <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="str">
-        <v>--</v>
+        <v>9000</v>
+      </c>
+      <c r="N6">
+        <v>30000</v>
       </c>
       <c r="O6">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve">222/RABAT </v>
-      </c>
-      <c r="B7" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C7" t="str">
-        <v>K2574857</v>
-      </c>
-      <c r="D7" t="str">
-        <v>NADIA JJEE</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
-      <c r="H7">
-        <v>13333.33</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>2000</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="str">
-        <v>--</v>
-      </c>
-      <c r="O7">
-        <v>11333.33</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v xml:space="preserve">222/RABAT </v>
-      </c>
-      <c r="B8" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C8" t="str">
-        <v>KL354654</v>
-      </c>
-      <c r="D8" t="str">
-        <v>MOUNIR NNNN</v>
-      </c>
-      <c r="E8" t="str">
-        <v>non</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>6666.67</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>666.67</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="str">
-        <v>--</v>
-      </c>
-      <c r="O8">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>800/PV FES 1</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C9" t="str">
-        <v>K5443645</v>
-      </c>
-      <c r="D9" t="str">
-        <v>KHADIJA LALA</v>
-      </c>
-      <c r="E9" t="str">
-        <v>non</v>
-      </c>
-      <c r="F9" t="str">
-        <v>trimestrielle</v>
-      </c>
-      <c r="G9">
-        <v>15</v>
-      </c>
-      <c r="H9">
-        <v>35000</v>
-      </c>
-      <c r="I9">
-        <v>35000</v>
-      </c>
-      <c r="J9">
-        <v>5250</v>
-      </c>
-      <c r="K9">
-        <v>5250</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="str">
-        <v>--</v>
-      </c>
-      <c r="O9">
-        <v>29750</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H10">
-        <v>83000</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>11276.67</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>16000</v>
-      </c>
-      <c r="M10">
-        <v>48000</v>
-      </c>
-      <c r="N10">
-        <v>7200</v>
-      </c>
-      <c r="O10">
-        <v>128523.33</v>
+        <v>157500</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>